<commit_message>
added steps with descriptions to UI and updated instructions
</commit_message>
<xml_diff>
--- a/inst/extdata/DataTemplate.xlsx
+++ b/inst/extdata/DataTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/PartTimers/Nick Lombardo/BMP/FWCCalculator/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{A796D49A-F9F1-43CF-9F05-6148105357BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEFA940D-D6BC-4543-8007-8ABD36EDC0A6}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{A796D49A-F9F1-43CF-9F05-6148105357BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A00FC129-B058-4FF4-8EA3-6F58EBBA6D14}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{151604A7-0CE7-4EA8-9370-ACC891023C94}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Flow (L/s)</t>
   </si>
@@ -55,19 +55,7 @@
     <t>This calculator will produce a table of aliquot volume values, a hydrograph, and, if pollutant data is provided, pollutograph(s) for the given data set of flow rate measurements and sample timestamps.</t>
   </si>
   <si>
-    <t>1. Download the Excel template file here and overwrite it with your data. See the Data Requirements section below.</t>
-  </si>
-  <si>
     <t xml:space="preserve">  NOTE: a 'download.htm' file may be downloaded instead of the template Excel file if the link is clicked too soon after launching the application. This is a known issue with the 'shiny' R package which was used to develop this application. Please allow a few minutes before downloading the template.</t>
-  </si>
-  <si>
-    <t>3. Use the 'Start Time' and 'End Time' inputs to filter the data to the appropriate time range. Elapsed time in minutes is presented. The grayed-out sections of the graph will not be included in the aliquot volume and event mean concentration calculations.</t>
-  </si>
-  <si>
-    <t>4. After changing the 'Start Time' and 'End Time', click the 'Redraw Graph(s)' button to regenerate the aliquot volume table, hydrograph, and pollutograph(s), filtered to the provided times.</t>
-  </si>
-  <si>
-    <t>5. The 'Composite Vol.' input is used in the aliquot volume calculation such that the sum of the aliquot volumes will be equal to the composite volume value entered here, measured in mL.</t>
   </si>
   <si>
     <t>6. The 'Flow Units of Submitted Data' input is used to label and calculate the 'Total Hydrograph Volume' output.</t>
@@ -77,9 +65,6 @@
   </si>
   <si>
     <t>The uploaded Excel spreadsheet must conform to the following requirements:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  * Must contain exactly two sheets, in the following order:</t>
   </si>
   <si>
     <t xml:space="preserve">    - Sheet 1: flow rate measurement data</t>
@@ -128,6 +113,27 @@
   </si>
   <si>
     <t xml:space="preserve">    If pollutant data is provided, the calculator will also provide the Event Mean Concentration for each of the specified pollutants.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  * Must contain exactly three sheets, in the following order:</t>
+  </si>
+  <si>
+    <t>7. Use the 'Reload App' button to submit a new data set.</t>
+  </si>
+  <si>
+    <t>1. Download the Excel template file and overwrite it with your data. See the Data Requirements section below.</t>
+  </si>
+  <si>
+    <t>3. Use the 'Start Date/Time' and 'End Date/Time' inputs to filter the data to the appropriate time range. The grayed-out sections of the graph will not be included in the aliquot volume and event mean concentration calculations.</t>
+  </si>
+  <si>
+    <t>4. After changing the 'Start Date/Time' and 'End Date/Time' inputs, click the 'Draw Graph(s)' button to regenerate the aliquot volume table, hydrograph, and pollutograph(s), filtered to the provided times.</t>
+  </si>
+  <si>
+    <t>5. The 'Composite Vol.' input is used in the aliquot volume calculation such that the sum of the aliquot volumes will be equal to the composite volume value entered here, measured in mL. The minimum and maximum supported values are 500 mL and 10,000 mL, respectively.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - Instructions: instructions for using the calculator</t>
   </si>
 </sst>
 </file>
@@ -216,10 +222,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FAF7B6-D860-44E6-BB57-F330BDC390ED}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -537,132 +539,142 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
+      <c r="A13" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3202,8 +3214,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21cacd0d90dbd8beb6fc12ad84d4cd0e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b418c8325abc32123734ac979891270" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="582b150a9eb9a8984bd6398cf909f49d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a4808acce3a6e68b39fbd804e31fb38" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
     <xsd:import namespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
@@ -3230,6 +3242,7 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3318,6 +3331,11 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="26" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -3462,15 +3480,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -3483,35 +3492,20 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAB9C9D5-B60E-41F9-9E50-B02621F3CF7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
-    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5648F7E3-2A96-42C1-B669-98075E2FB631}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B490D82-BD57-4D10-9D7F-A45C282EA46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EF85FC7-95A8-4336-A444-88BFC7E32339}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3521,4 +3515,12 @@
     <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B490D82-BD57-4D10-9D7F-A45C282EA46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added check for duplicated data and more than one storm event, updated instructions to specify one storm event
</commit_message>
<xml_diff>
--- a/inst/extdata/DataTemplate.xlsx
+++ b/inst/extdata/DataTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/PartTimers/Nick Lombardo/BMP/FWCCalculator/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/NickLombardo/BMP/FWCCalculator/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{A796D49A-F9F1-43CF-9F05-6148105357BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A00FC129-B058-4FF4-8EA3-6F58EBBA6D14}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{A796D49A-F9F1-43CF-9F05-6148105357BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6479FA9-9491-4742-ABD7-499C423323DF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{151604A7-0CE7-4EA8-9370-ACC891023C94}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{151604A7-0CE7-4EA8-9370-ACC891023C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Flow (L/s)</t>
   </si>
@@ -103,9 +103,6 @@
     <t xml:space="preserve">  * The column headers are required and can be renamed as needed, but cannot be exclusively numeric characters [0-9].</t>
   </si>
   <si>
-    <t xml:space="preserve">  * All flow rate and pollutant measurements must be greater than zero.</t>
-  </si>
-  <si>
     <t xml:space="preserve">  * There may not be any missing values in the spreadsheet.</t>
   </si>
   <si>
@@ -134,6 +131,12 @@
   </si>
   <si>
     <t xml:space="preserve">    - Instructions: instructions for using the calculator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  * Must contain data for exactly one storm event.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  * All flow rate and pollutant measurements must be greater than or equal to zero.</t>
   </si>
 </sst>
 </file>
@@ -222,6 +225,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,160 +528,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FAF7B6-D860-44E6-BB57-F330BDC390ED}">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -689,13 +703,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -703,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>39976.397222222222</v>
       </c>
@@ -711,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>39976.398611111108</v>
       </c>
@@ -719,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>39976.400000000001</v>
       </c>
@@ -727,7 +741,7 @@
         <v>1.8186080586080587E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>39976.401388888888</v>
       </c>
@@ -735,7 +749,7 @@
         <v>6.3651282051282052E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>39976.402777777781</v>
       </c>
@@ -743,7 +757,7 @@
         <v>0.1454886446886447</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>39976.404166666667</v>
       </c>
@@ -751,7 +765,7 @@
         <v>0.26483479853479858</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>39976.405555555553</v>
       </c>
@@ -759,7 +773,7 @@
         <v>0.32962271062271065</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>39976.406944444447</v>
       </c>
@@ -767,7 +781,7 @@
         <v>0.28529413919413921</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>39976.408333333333</v>
       </c>
@@ -775,7 +789,7 @@
         <v>0.28302087912087909</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>39976.409722222219</v>
       </c>
@@ -783,7 +797,7 @@
         <v>0.39100073260073259</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>39976.411111111112</v>
       </c>
@@ -791,7 +805,7 @@
         <v>0.48306776556776554</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>39976.412499999999</v>
       </c>
@@ -799,7 +813,7 @@
         <v>0.42850952380952378</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>39976.413888888892</v>
       </c>
@@ -807,7 +821,7 @@
         <v>0.30916336996336996</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>39976.415277777778</v>
       </c>
@@ -815,7 +829,7 @@
         <v>0.1773142857142857</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>39976.416666666664</v>
       </c>
@@ -823,7 +837,7 @@
         <v>0.11138974358974359</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>39976.418055555558</v>
       </c>
@@ -831,7 +845,7 @@
         <v>6.7061172161172161E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>39976.419444444444</v>
       </c>
@@ -839,7 +853,7 @@
         <v>4.2055311355311355E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>39976.42083333333</v>
       </c>
@@ -847,7 +861,7 @@
         <v>2.5005860805860806E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>39976.422222222223</v>
       </c>
@@ -855,7 +869,7 @@
         <v>1.5912820512820513E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>39976.423611111109</v>
       </c>
@@ -863,7 +877,7 @@
         <v>0.19095384615384614</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>39976.425000000003</v>
       </c>
@@ -871,7 +885,7 @@
         <v>0.77404505494505482</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>39976.426388888889</v>
       </c>
@@ -879,7 +893,7 @@
         <v>1.4230608058608059</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>39976.427777777775</v>
       </c>
@@ -887,7 +901,7 @@
         <v>1.5992384615384614</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>39976.429166666669</v>
       </c>
@@ -895,7 +909,7 @@
         <v>1.3150809523809524</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>39976.430555555555</v>
       </c>
@@ -903,7 +917,7 @@
         <v>0.85815567765567768</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>39976.431944444441</v>
       </c>
@@ -911,7 +925,7 @@
         <v>0.51148351648351642</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>39976.433333333334</v>
       </c>
@@ -919,7 +933,7 @@
         <v>0.31484652014652009</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>39976.43472222222</v>
       </c>
@@ -927,7 +941,7 @@
         <v>0.19322710622710623</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>39976.436111111114</v>
       </c>
@@ -935,7 +949,7 @@
         <v>0.11820952380952381</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>39976.4375</v>
       </c>
@@ -943,7 +957,7 @@
         <v>7.2744322344322349E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>39976.438888888886</v>
       </c>
@@ -951,7 +965,7 @@
         <v>4.5465201465201471E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>39976.44027777778</v>
       </c>
@@ -959,7 +973,7 @@
         <v>2.7279120879120877E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>39976.441666666666</v>
       </c>
@@ -967,7 +981,7 @@
         <v>1.7049450549450552E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>39976.443055555559</v>
       </c>
@@ -975,7 +989,7 @@
         <v>1.0229670329670329E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>39976.444444444445</v>
       </c>
@@ -983,7 +997,7 @@
         <v>5.6831501831501839E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>39976.445833333331</v>
       </c>
@@ -991,7 +1005,7 @@
         <v>1.1366300366300367E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>39976.447222222225</v>
       </c>
@@ -999,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>39976.448611111111</v>
       </c>
@@ -1007,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39976.449999999997</v>
       </c>
@@ -1015,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>39976.451388888891</v>
       </c>
@@ -1023,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>39976.452777777777</v>
       </c>
@@ -1031,7 +1045,7 @@
         <v>0.15117179487179488</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>39976.45416666667</v>
       </c>
@@ -1039,7 +1053,7 @@
         <v>0.52739633699633692</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>39976.455555555556</v>
       </c>
@@ -1047,7 +1061,7 @@
         <v>0.78995787545787555</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>39976.456944444442</v>
       </c>
@@ -1055,7 +1069,7 @@
         <v>0.74221941391941393</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>39976.458333333336</v>
       </c>
@@ -1063,7 +1077,7 @@
         <v>0.54330915750915754</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>39976.459722222222</v>
       </c>
@@ -1071,7 +1085,7 @@
         <v>0.47738461538461546</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>39976.461111111108</v>
       </c>
@@ -1079,7 +1093,7 @@
         <v>0.77177179487179493</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>39976.462500000001</v>
       </c>
@@ -1087,7 +1101,7 @@
         <v>0.98318498168498158</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>39976.463888888888</v>
       </c>
@@ -1095,7 +1109,7 @@
         <v>1.0661589743589743</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>39976.465277777781</v>
       </c>
@@ -1103,7 +1117,7 @@
         <v>1.2605227106227106</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>39976.466666666667</v>
       </c>
@@ -1111,7 +1125,7 @@
         <v>1.3014413919413919</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>39976.468055555553</v>
       </c>
@@ -1119,7 +1133,7 @@
         <v>1.2957582417582418</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>39976.469444444447</v>
       </c>
@@ -1127,7 +1141,7 @@
         <v>1.4401102564102564</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>39976.470833333333</v>
       </c>
@@ -1135,7 +1149,7 @@
         <v>1.4457934065934068</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>39976.472222222219</v>
       </c>
@@ -1143,7 +1157,7 @@
         <v>1.2139208791208791</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>39976.473611111112</v>
       </c>
@@ -1151,7 +1165,7 @@
         <v>0.85133589743589733</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>39976.474999999999</v>
       </c>
@@ -1159,7 +1173,7 @@
         <v>0.49557069597069592</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>39976.476388888892</v>
       </c>
@@ -1167,7 +1181,7 @@
         <v>0.5080736263736263</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>39976.477777777778</v>
       </c>
@@ -1175,7 +1189,7 @@
         <v>0.88316153846153855</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>39976.479166666664</v>
       </c>
@@ -1183,7 +1197,7 @@
         <v>1.1604992673992673</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>39976.480555555558</v>
       </c>
@@ -1191,7 +1205,7 @@
         <v>1.0502461538461538</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>39976.481944444444</v>
       </c>
@@ -1199,7 +1213,7 @@
         <v>0.76040549450549455</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>39976.48333333333</v>
       </c>
@@ -1207,7 +1221,7 @@
         <v>0.6467424908424908</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>39976.484722222223</v>
       </c>
@@ -1215,7 +1229,7 @@
         <v>1.0002344322344321</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>39976.486111111109</v>
       </c>
@@ -1223,7 +1237,7 @@
         <v>1.2548395604395604</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>39976.487500000003</v>
       </c>
@@ -1231,7 +1245,7 @@
         <v>1.3457699633699634</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>39976.488888888889</v>
       </c>
@@ -1239,7 +1253,7 @@
         <v>1.5662761904761906</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>39976.490277777775</v>
       </c>
@@ -1247,7 +1261,7 @@
         <v>1.8265644688644689</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>39976.491666666669</v>
       </c>
@@ -1255,7 +1269,7 @@
         <v>2.1391377289377291</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>39976.493055555555</v>
       </c>
@@ -1263,7 +1277,7 @@
         <v>2.1277714285714286</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>39976.494444444441</v>
       </c>
@@ -1271,7 +1285,7 @@
         <v>1.6583432234432236</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>39976.495833333334</v>
       </c>
@@ -1279,7 +1293,7 @@
         <v>1.3832787545787546</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>39976.49722222222</v>
       </c>
@@ -1287,7 +1301,7 @@
         <v>1.4764824175824174</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>39976.498611111114</v>
       </c>
@@ -1295,7 +1309,7 @@
         <v>1.8640732600732601</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>39976.5</v>
       </c>
@@ -1303,7 +1317,7 @@
         <v>2.2130186813186818</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>39976.501388888886</v>
       </c>
@@ -1311,7 +1325,7 @@
         <v>2.2277948717948717</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>39976.50277777778</v>
       </c>
@@ -1319,7 +1333,7 @@
         <v>1.7356340659340659</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>39976.504166666666</v>
       </c>
@@ -1327,7 +1341,7 @@
         <v>1.4514765567765568</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>39976.505555555559</v>
       </c>
@@ -1335,7 +1349,7 @@
         <v>1.5469534798534799</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>39976.506944444445</v>
       </c>
@@ -1343,7 +1357,7 @@
         <v>1.9561402930402929</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>39976.508333333331</v>
       </c>
@@ -1351,7 +1365,7 @@
         <v>2.3175886446886445</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>39976.509722222225</v>
       </c>
@@ -1359,7 +1373,7 @@
         <v>2.5835600732600734</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>39976.511111111111</v>
       </c>
@@ -1367,7 +1381,7 @@
         <v>2.6926765567765565</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>39976.512499999997</v>
       </c>
@@ -1375,7 +1389,7 @@
         <v>2.8381652014652015</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>39976.513888888891</v>
       </c>
@@ -1383,7 +1397,7 @@
         <v>2.8677175824175829</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>39976.515277777777</v>
       </c>
@@ -1391,7 +1405,7 @@
         <v>2.9688776556776557</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>39976.51666666667</v>
       </c>
@@ -1399,7 +1413,7 @@
         <v>2.9631945054945055</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>39976.518055555556</v>
       </c>
@@ -1407,7 +1421,7 @@
         <v>2.7801970695970697</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>39976.519444444442</v>
       </c>
@@ -1415,7 +1429,7 @@
         <v>2.3698736263736264</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>39976.520833333336</v>
       </c>
@@ -1423,7 +1437,7 @@
         <v>2.3721468864468864</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>39976.522222222222</v>
       </c>
@@ -1431,7 +1445,7 @@
         <v>2.4960395604395602</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>39976.523611111108</v>
       </c>
@@ -1439,7 +1453,7 @@
         <v>2.7597377289377287</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>39976.525000000001</v>
       </c>
@@ -1447,7 +1461,7 @@
         <v>2.9359153846153845</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>39976.526388888888</v>
       </c>
@@ -1455,7 +1469,7 @@
         <v>3.2723578754578755</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>39976.527777777781</v>
       </c>
@@ -1463,7 +1477,7 @@
         <v>3.7861146520146525</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>39976.529166666667</v>
       </c>
@@ -1471,7 +1485,7 @@
         <v>3.8634054945054941</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>39976.530555555553</v>
       </c>
@@ -1479,7 +1493,7 @@
         <v>4.0714087912087908</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>39976.531944444447</v>
       </c>
@@ -1487,7 +1501,7 @@
         <v>4.2623626373626378</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>39976.533333333333</v>
       </c>
@@ -1495,7 +1509,7 @@
         <v>4.1987113553113549</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>39976.534722222219</v>
       </c>
@@ -1503,7 +1517,7 @@
         <v>4.2998714285714286</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>39976.536111111112</v>
       </c>
@@ -1511,7 +1525,7 @@
         <v>4.9170615384615388</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>39976.537499999999</v>
       </c>
@@ -1519,7 +1533,7 @@
         <v>5.9911769230769236</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>39976.538888888892</v>
       </c>
@@ -1527,7 +1541,7 @@
         <v>6.912983882783883</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>39976.540277777778</v>
       </c>
@@ -1535,7 +1549,7 @@
         <v>7.190321611721612</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>39976.541666666664</v>
       </c>
@@ -1543,7 +1557,7 @@
         <v>7.1698622710622715</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>39976.543055555558</v>
       </c>
@@ -1551,7 +1565,7 @@
         <v>7.0300567765567772</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>39976.544444444444</v>
       </c>
@@ -1559,7 +1573,7 @@
         <v>7.1925948717948724</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>39976.54583333333</v>
       </c>
@@ -1567,7 +1581,7 @@
         <v>7.8654798534798527</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>39976.547222222223</v>
       </c>
@@ -1575,7 +1589,7 @@
         <v>8.7134058608058602</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>39976.548611111109</v>
       </c>
@@ -1583,7 +1597,7 @@
         <v>9.0168860805860795</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>39976.550000000003</v>
       </c>
@@ -1591,7 +1605,7 @@
         <v>8.4178820512820511</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>39976.551388888889</v>
       </c>
@@ -1599,7 +1613,7 @@
         <v>7.1266703296703291</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>39976.552777777775</v>
       </c>
@@ -1607,7 +1621,7 @@
         <v>5.8627377289377298</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>39976.554166666669</v>
       </c>
@@ -1615,7 +1629,7 @@
         <v>4.6670029304029308</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>39976.555555555555</v>
       </c>
@@ -1623,7 +1637,7 @@
         <v>3.6394893772893773</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>39976.556944444441</v>
       </c>
@@ -1631,7 +1645,7 @@
         <v>3.2780410256410253</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>39976.558333333334</v>
       </c>
@@ -1639,7 +1653,7 @@
         <v>2.8972699633699635</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>39976.55972222222</v>
       </c>
@@ -1647,7 +1661,7 @@
         <v>2.3005391941391942</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>39976.561111111114</v>
       </c>
@@ -1655,7 +1669,7 @@
         <v>1.8822593406593406</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>39976.5625</v>
       </c>
@@ -1663,7 +1677,7 @@
         <v>1.9845560439560441</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>39976.563888888886</v>
       </c>
@@ -1671,7 +1685,7 @@
         <v>2.1584604395604399</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>39976.56527777778</v>
       </c>
@@ -1679,7 +1693,7 @@
         <v>2.1414109890109891</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
         <v>39976.566666666666</v>
       </c>
@@ -1687,7 +1701,7 @@
         <v>2.3596439560439562</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>39976.568055555559</v>
       </c>
@@ -1695,7 +1709,7 @@
         <v>2.3391846153846152</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>39976.569444444445</v>
       </c>
@@ -1703,7 +1717,7 @@
         <v>1.9606868131868129</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>39976.570833333331</v>
       </c>
@@ -1711,7 +1725,7 @@
         <v>1.6788025641025641</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>39976.572222222225</v>
       </c>
@@ -1719,7 +1733,7 @@
         <v>1.8640732600732601</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>39976.573611111111</v>
       </c>
@@ -1727,7 +1741,7 @@
         <v>2.3994260073260074</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>39976.574999999997</v>
       </c>
@@ -1735,7 +1749,7 @@
         <v>2.8699908424908425</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>39976.576388888891</v>
       </c>
@@ -1743,7 +1757,7 @@
         <v>2.8847670329670332</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>39976.577777777777</v>
       </c>
@@ -1751,7 +1765,7 @@
         <v>2.2437076923076922</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>39976.57916666667</v>
       </c>
@@ -1759,7 +1773,7 @@
         <v>1.8708930402930404</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>39976.580555555556</v>
       </c>
@@ -1767,7 +1781,7 @@
         <v>1.9811461538461537</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>39976.581944444442</v>
       </c>
@@ -1775,7 +1789,7 @@
         <v>2.4824000000000002</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>39976.583333333336</v>
       </c>
@@ -1783,7 +1797,7 @@
         <v>2.9211391941391942</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>39976.584722222222</v>
       </c>
@@ -1791,7 +1805,7 @@
         <v>3.2359857142857145</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>39976.586111111108</v>
       </c>
@@ -1799,7 +1813,7 @@
         <v>3.3462388278388278</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>39976.587500000001</v>
       </c>
@@ -1807,7 +1821,7 @@
         <v>3.1916571428571427</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>39976.588888888888</v>
       </c>
@@ -1815,7 +1829,7 @@
         <v>2.7449615384615385</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>39976.590277777781</v>
       </c>
@@ -1823,7 +1837,7 @@
         <v>2.760874358974359</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>39976.591666666667</v>
       </c>
@@ -1831,7 +1845,7 @@
         <v>2.5960630036630037</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>39976.593055555553</v>
       </c>
@@ -1839,7 +1853,7 @@
         <v>2.1311813186813189</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="3">
         <v>39976.594444444447</v>
       </c>
@@ -1847,7 +1861,7 @@
         <v>1.7879190476190476</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>39976.595833333333</v>
       </c>
@@ -1855,7 +1869,7 @@
         <v>1.9447739926739929</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>39976.597222222219</v>
       </c>
@@ -1863,7 +1877,7 @@
         <v>2.1550505494505496</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>39976.598611111112</v>
       </c>
@@ -1871,7 +1885,7 @@
         <v>1.8481604395604396</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
         <v>39976.6</v>
       </c>
@@ -1879,7 +1893,7 @@
         <v>1.3139443223443223</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>39976.601388888892</v>
       </c>
@@ -1887,7 +1901,7 @@
         <v>0.75699560439560443</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>39976.602777777778</v>
       </c>
@@ -1895,7 +1909,7 @@
         <v>0.47283809523809522</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>39976.604166666664</v>
       </c>
@@ -1903,7 +1917,7 @@
         <v>0.28302087912087909</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
         <v>39976.605555555558</v>
       </c>
@@ -1911,7 +1925,7 @@
         <v>0.17504102564102564</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>39976.606944444444</v>
       </c>
@@ -1919,7 +1933,7 @@
         <v>0.10343333333333334</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>39976.60833333333</v>
       </c>
@@ -1927,7 +1941,7 @@
         <v>6.5924542124542115E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>39976.609722222223</v>
       </c>
@@ -1935,7 +1949,7 @@
         <v>3.7508791208791213E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="3">
         <v>39976.611111111109</v>
       </c>
@@ -1943,7 +1957,7 @@
         <v>2.1595970695970693E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>39976.612500000003</v>
       </c>
@@ -1951,7 +1965,7 @@
         <v>1.3639560439560439E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>39976.613888888889</v>
       </c>
@@ -1959,7 +1973,7 @@
         <v>7.9564102564102564E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>39976.615277777775</v>
       </c>
@@ -1967,7 +1981,7 @@
         <v>3.4098901098901097E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="3">
         <v>39976.616666666669</v>
       </c>
@@ -1975,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>39976.618055555555</v>
       </c>
@@ -1983,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>39976.619444444441</v>
       </c>
@@ -1991,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>39976.620833333334</v>
       </c>
@@ -1999,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="3">
         <v>39976.62222222222</v>
       </c>
@@ -2007,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>39976.623611111114</v>
       </c>
@@ -2015,1105 +2029,1105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="3"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="3"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="3"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="3"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="3"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="3"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="3"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="3"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="3"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="3"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" s="3"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" s="3"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" s="3"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" s="3"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" s="3"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" s="3"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" s="3"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" s="3"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" s="3"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" s="3"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" s="3"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" s="3"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" s="3"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" s="3"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" s="3"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" s="3"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" s="3"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" s="3"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" s="3"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" s="3"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" s="3"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" s="3"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" s="3"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" s="3"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" s="3"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" s="3"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" s="3"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" s="3"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" s="3"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" s="3"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" s="3"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" s="3"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" s="3"/>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" s="3"/>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" s="3"/>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" s="3"/>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" s="3"/>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" s="3"/>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" s="3"/>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" s="3"/>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" s="3"/>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" s="3"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" s="3"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" s="3"/>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" s="3"/>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" s="3"/>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" s="3"/>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" s="3"/>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" s="3"/>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" s="3"/>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" s="3"/>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" s="3"/>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" s="3"/>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" s="3"/>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" s="3"/>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" s="3"/>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" s="3"/>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" s="3"/>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" s="3"/>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" s="3"/>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" s="3"/>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" s="3"/>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" s="3"/>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" s="3"/>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" s="3"/>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" s="3"/>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" s="3"/>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" s="3"/>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" s="3"/>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" s="3"/>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" s="3"/>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" s="3"/>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" s="3"/>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" s="3"/>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" s="3"/>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" s="3"/>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" s="3"/>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" s="3"/>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" s="3"/>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" s="3"/>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" s="3"/>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" s="3"/>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" s="3"/>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" s="3"/>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" s="3"/>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" s="3"/>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" s="3"/>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" s="3"/>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" s="3"/>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" s="3"/>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" s="3"/>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" s="3"/>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" s="3"/>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" s="3"/>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" s="3"/>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" s="3"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" s="3"/>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" s="3"/>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" s="3"/>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" s="3"/>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" s="3"/>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" s="3"/>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" s="3"/>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" s="3"/>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" s="3"/>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" s="3"/>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" s="3"/>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" s="3"/>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" s="3"/>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" s="3"/>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" s="3"/>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" s="3"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" s="3"/>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" s="3"/>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" s="3"/>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" s="3"/>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" s="3"/>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" s="3"/>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" s="3"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" s="3"/>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" s="3"/>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" s="3"/>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" s="3"/>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" s="3"/>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" s="3"/>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A302" s="3"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A303" s="3"/>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A304" s="3"/>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A305" s="3"/>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A306" s="3"/>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A307" s="3"/>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A308" s="3"/>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A309" s="3"/>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A310" s="3"/>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A311" s="3"/>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A312" s="3"/>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A313" s="3"/>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A314" s="3"/>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A315" s="3"/>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A316" s="3"/>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A317" s="3"/>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A318" s="3"/>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A319" s="3"/>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A320" s="3"/>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" s="3"/>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" s="3"/>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" s="3"/>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" s="3"/>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" s="3"/>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" s="3"/>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" s="3"/>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" s="3"/>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" s="3"/>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" s="3"/>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" s="3"/>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" s="3"/>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" s="3"/>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" s="3"/>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" s="3"/>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" s="3"/>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" s="3"/>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" s="3"/>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" s="3"/>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" s="3"/>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" s="3"/>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" s="3"/>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" s="3"/>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" s="3"/>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" s="3"/>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" s="3"/>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" s="3"/>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" s="3"/>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" s="3"/>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" s="3"/>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" s="3"/>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" s="3"/>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" s="3"/>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" s="3"/>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" s="3"/>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" s="3"/>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" s="3"/>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" s="3"/>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" s="3"/>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" s="3"/>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" s="3"/>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" s="3"/>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" s="3"/>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" s="3"/>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" s="3"/>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A366" s="3"/>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A367" s="3"/>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A368" s="3"/>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A369" s="3"/>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A370" s="3"/>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A371" s="3"/>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A372" s="3"/>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A373" s="3"/>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A374" s="3"/>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A375" s="3"/>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A376" s="3"/>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A377" s="3"/>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A378" s="3"/>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A379" s="3"/>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A380" s="3"/>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A381" s="3"/>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A382" s="3"/>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A383" s="3"/>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A384" s="3"/>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A385" s="3"/>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A386" s="3"/>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A387" s="3"/>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A388" s="3"/>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A389" s="3"/>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A390" s="3"/>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A391" s="3"/>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A392" s="3"/>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A393" s="3"/>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A394" s="3"/>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A395" s="3"/>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A396" s="3"/>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A397" s="3"/>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A398" s="3"/>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A399" s="3"/>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A400" s="3"/>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A401" s="3"/>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A402" s="3"/>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A403" s="3"/>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A404" s="3"/>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A405" s="3"/>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A406" s="3"/>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A407" s="3"/>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A408" s="3"/>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A409" s="3"/>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A410" s="3"/>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A411" s="3"/>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A412" s="3"/>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A413" s="3"/>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A414" s="3"/>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A415" s="3"/>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A416" s="3"/>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A417" s="3"/>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A418" s="3"/>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A419" s="3"/>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A420" s="3"/>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A421" s="3"/>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A422" s="3"/>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A423" s="3"/>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A424" s="3"/>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A425" s="3"/>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A426" s="3"/>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A427" s="3"/>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A428" s="3"/>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A429" s="3"/>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A430" s="3"/>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A431" s="3"/>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A432" s="3"/>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A433" s="3"/>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A434" s="3"/>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A435" s="3"/>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A436" s="3"/>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A437" s="3"/>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A438" s="3"/>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A439" s="3"/>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A440" s="3"/>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A441" s="3"/>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A442" s="3"/>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A443" s="3"/>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A444" s="3"/>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A445" s="3"/>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A446" s="3"/>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A447" s="3"/>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A448" s="3"/>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A449" s="3"/>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A450" s="3"/>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A451" s="3"/>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A452" s="3"/>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A453" s="3"/>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A454" s="3"/>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A455" s="3"/>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A456" s="3"/>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A457" s="3"/>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A458" s="3"/>
     </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A459" s="3"/>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A460" s="3"/>
     </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A461" s="3"/>
     </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A462" s="3"/>
     </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A463" s="3"/>
     </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A464" s="3"/>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A465" s="3"/>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A466" s="3"/>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A467" s="3"/>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A468" s="3"/>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A469" s="3"/>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A470" s="3"/>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A471" s="3"/>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A472" s="3"/>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A473" s="3"/>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A474" s="3"/>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A475" s="3"/>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A476" s="3"/>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A477" s="3"/>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A478" s="3"/>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A479" s="3"/>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A480" s="3"/>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A481" s="3"/>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A482" s="3"/>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A483" s="3"/>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A484" s="3"/>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A485" s="3"/>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A486" s="3"/>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A487" s="3"/>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A488" s="3"/>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A489" s="3"/>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A490" s="3"/>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A491" s="3"/>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A492" s="3"/>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A493" s="3"/>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A494" s="3"/>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A495" s="3"/>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A496" s="3"/>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A497" s="3"/>
     </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A498" s="3"/>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A499" s="3"/>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A500" s="3"/>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A501" s="3"/>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A502" s="3"/>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A503" s="3"/>
     </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A504" s="3"/>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A505" s="3"/>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A506" s="3"/>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A507" s="3"/>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A508" s="3"/>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A509" s="3"/>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A510" s="3"/>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A511" s="3"/>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A512" s="3"/>
     </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A513" s="3"/>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A514" s="3"/>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A515" s="3"/>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A516" s="3"/>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A517" s="3"/>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A518" s="3"/>
     </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A519" s="3"/>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A520" s="3"/>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A521" s="3"/>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A522" s="3"/>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A523" s="3"/>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A524" s="3"/>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A525" s="3"/>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A526" s="3"/>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A527" s="3"/>
     </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A528" s="3"/>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A529" s="3"/>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A530" s="3"/>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A531" s="3"/>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A532" s="3"/>
     </row>
   </sheetData>
@@ -3128,13 +3142,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3142,7 +3156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>39976.533333333333</v>
       </c>
@@ -3150,7 +3164,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>39976.537499999999</v>
       </c>
@@ -3158,7 +3172,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>39976.541666666664</v>
       </c>
@@ -3166,7 +3180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>39976.54583333333</v>
       </c>
@@ -3174,7 +3188,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>39976.552777777775</v>
       </c>
@@ -3182,7 +3196,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>39976.55972222222</v>
       </c>
@@ -3190,7 +3204,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>39976.587500000001</v>
       </c>
@@ -3198,13 +3212,13 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
   </sheetData>
@@ -3214,8 +3228,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="582b150a9eb9a8984bd6398cf909f49d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a4808acce3a6e68b39fbd804e31fb38" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75e20f4bf570a29fdd68b6ac0ce9f23e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d8333fcdd8157586878df4d15f204f2" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
     <xsd:import namespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
@@ -3243,6 +3257,7 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:OldForms" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3336,6 +3351,13 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="26" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OldForms" ma:index="27" nillable="true" ma:displayName="Old Forms " ma:format="Dropdown" ma:internalName="OldForms">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -3488,6 +3510,7 @@
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
     <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
+    <OldForms xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
@@ -3502,17 +3525,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5648F7E3-2A96-42C1-B669-98075E2FB631}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60F2C54A-3816-4A41-AF43-6087780B2184}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
+    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EF85FC7-95A8-4336-A444-88BFC7E32339}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
-    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>